<commit_message>
docs: add new doc about error handling
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsErrors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25B8F2B6-BFA1-B94D-9057-8CEAC2D6E94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3A282F-2D06-4BBD-B2F0-234D328FDE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -494,12 +494,12 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>253</v>
       </c>
@@ -554,7 +554,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>253</v>
       </c>
@@ -580,7 +580,7 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>253</v>
       </c>
@@ -606,7 +606,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>253</v>
       </c>
@@ -632,7 +632,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>253</v>
       </c>
@@ -658,7 +658,7 @@
         <v>0.79166666666666696</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
@@ -681,7 +681,7 @@
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>253</v>
       </c>
@@ -707,7 +707,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>253</v>
       </c>
@@ -733,7 +733,7 @@
         <v>0.91666666666666696</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>253</v>
       </c>
@@ -759,7 +759,7 @@
         <v>0.95833333333333304</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>253</v>
       </c>
@@ -785,7 +785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>253</v>
       </c>
@@ -811,7 +811,7 @@
         <v>1.0416666666666701</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>253</v>
       </c>
@@ -822,7 +822,7 @@
         <v>20</v>
       </c>
       <c r="D13">
-        <v>23.56</v>
+        <v>1000000</v>
       </c>
       <c r="E13" s="1">
         <v>45255</v>
@@ -837,7 +837,7 @@
         <v>1.0833333333333299</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2</v>
       </c>
@@ -860,7 +860,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>253</v>
       </c>
@@ -886,7 +886,7 @@
         <v>1.1666666666666701</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>253</v>
       </c>

</xml_diff>

<commit_message>
feat: improve checks for integer values
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsErrors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3A282F-2D06-4BBD-B2F0-234D328FDE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D566F5-4946-4892-A62A-9F11EBEB613C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5475" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>24.56</t>
+  </si>
+  <si>
+    <t>2 EUR</t>
   </si>
 </sst>
 </file>
@@ -148,10 +151,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -494,10 +498,13 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -636,8 +643,8 @@
       <c r="A6">
         <v>253</v>
       </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="B6" s="3">
+        <v>2.5</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -712,7 +719,7 @@
         <v>253</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -737,8 +744,8 @@
       <c r="A10">
         <v>253</v>
       </c>
-      <c r="B10">
-        <v>2</v>
+      <c r="B10" t="s">
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
feat: add type checks for all EDM Types
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsErrors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D566F5-4946-4892-A62A-9F11EBEB613C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73017C7-4E74-443D-9F94-5EE66486D326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -110,6 +110,30 @@
   </si>
   <si>
     <t>2 EUR</t>
+  </si>
+  <si>
+    <t>Product Test 16</t>
+  </si>
+  <si>
+    <t>23.11.2023456</t>
+  </si>
+  <si>
+    <t>Product Test 17</t>
+  </si>
+  <si>
+    <t>23.11.2023457</t>
+  </si>
+  <si>
+    <t>Product Test 18</t>
+  </si>
+  <si>
+    <t>23.11.2023458</t>
+  </si>
+  <si>
+    <t>25.11.202312</t>
+  </si>
+  <si>
+    <t>24.11.202312</t>
   </si>
 </sst>
 </file>
@@ -151,11 +175,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -495,15 +520,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="9" max="9" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -918,6 +945,96 @@
       <c r="H16" s="2">
         <v>1.2083333333333299</v>
       </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>253</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>27.56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45254</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>253</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18">
+        <v>28.56</v>
+      </c>
+      <c r="E18" s="1">
+        <v>45255</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.2916666666666701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>253</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>29.56</v>
+      </c>
+      <c r="E19" s="1">
+        <v>45255</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45254</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2.041666666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fix: checking time values
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsErrors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73017C7-4E74-443D-9F94-5EE66486D326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D29A68A-BCF5-4709-910E-07E551FCDA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -175,12 +175,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -523,7 +522,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -917,7 +916,7 @@
         <v>45253</v>
       </c>
       <c r="H15" s="2">
-        <v>1.1666666666666701</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -943,7 +942,7 @@
         <v>45253</v>
       </c>
       <c r="H16" s="2">
-        <v>1.2083333333333299</v>
+        <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -969,7 +968,7 @@
         <v>31</v>
       </c>
       <c r="H17" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1020,7 +1019,7 @@
       <c r="G19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19">
         <v>2.041666666666667</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: improve checks for all Edm Types (#105)
* feat: improve checks for integer values

* chore: define ts types

* feat: add type checks for all EDM Types

* fix: time parsing

* fix: checking time values
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsErrors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3A282F-2D06-4BBD-B2F0-234D328FDE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D29A68A-BCF5-4709-910E-07E551FCDA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -107,6 +107,33 @@
   </si>
   <si>
     <t>24.56</t>
+  </si>
+  <si>
+    <t>2 EUR</t>
+  </si>
+  <si>
+    <t>Product Test 16</t>
+  </si>
+  <si>
+    <t>23.11.2023456</t>
+  </si>
+  <si>
+    <t>Product Test 17</t>
+  </si>
+  <si>
+    <t>23.11.2023457</t>
+  </si>
+  <si>
+    <t>Product Test 18</t>
+  </si>
+  <si>
+    <t>23.11.2023458</t>
+  </si>
+  <si>
+    <t>25.11.202312</t>
+  </si>
+  <si>
+    <t>24.11.202312</t>
   </si>
 </sst>
 </file>
@@ -148,10 +175,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -491,13 +519,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="9" max="9" width="17.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -636,8 +669,8 @@
       <c r="A6">
         <v>253</v>
       </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="B6" s="3">
+        <v>2.5</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -712,7 +745,7 @@
         <v>253</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -737,8 +770,8 @@
       <c r="A10">
         <v>253</v>
       </c>
-      <c r="B10">
-        <v>2</v>
+      <c r="B10" t="s">
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -883,7 +916,7 @@
         <v>45253</v>
       </c>
       <c r="H15" s="2">
-        <v>1.1666666666666701</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -909,8 +942,98 @@
         <v>45253</v>
       </c>
       <c r="H16" s="2">
-        <v>1.2083333333333299</v>
-      </c>
+        <v>0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>253</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>27.56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45254</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>253</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18">
+        <v>28.56</v>
+      </c>
+      <c r="E18" s="1">
+        <v>45255</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.2916666666666701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>253</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>29.56</v>
+      </c>
+      <c r="E19" s="1">
+        <v>45255</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45254</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19">
+        <v>2.041666666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fix: csv import dates
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsErrors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13801231-C7C7-4AB4-AAFD-E743903776F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAF8758-2D58-DC43-AECB-DDA82B34CD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="5820" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="4140" windowWidth="21600" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Product Test 1</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>WRONGCOLUMN[TEST]</t>
+  </si>
+  <si>
+    <t>05/14/2021</t>
   </si>
 </sst>
 </file>
@@ -522,17 +525,17 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:H1"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="9" max="9" width="17.875" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -561,7 +564,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -587,7 +590,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>253</v>
       </c>
@@ -613,7 +616,7 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>253</v>
       </c>
@@ -639,7 +642,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>253</v>
       </c>
@@ -665,7 +668,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>253</v>
       </c>
@@ -691,7 +694,7 @@
         <v>0.79166666666666696</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -714,7 +717,7 @@
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>253</v>
       </c>
@@ -740,7 +743,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>253</v>
       </c>
@@ -766,7 +769,7 @@
         <v>0.91666666666666696</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>253</v>
       </c>
@@ -792,7 +795,7 @@
         <v>0.95833333333333304</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>253</v>
       </c>
@@ -818,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>253</v>
       </c>
@@ -844,7 +847,7 @@
         <v>1.0416666666666701</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>253</v>
       </c>
@@ -870,7 +873,7 @@
         <v>1.0833333333333299</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>2</v>
       </c>
@@ -893,7 +896,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>253</v>
       </c>
@@ -919,7 +922,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>253</v>
       </c>
@@ -932,8 +935,8 @@
       <c r="D16">
         <v>26.56</v>
       </c>
-      <c r="E16" s="1">
-        <v>45255</v>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F16" s="1">
         <v>45254</v>
@@ -945,7 +948,7 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>253</v>
       </c>
@@ -971,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>253</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>1.2916666666666701</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>253</v>
       </c>
@@ -1023,13 +1026,13 @@
         <v>2.041666666666667</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>

</xml_diff>

<commit_message>
feat: show faulty value in the error dialog (#197)
* chore: update ui5 versions

* feat: extract more metadata out of excel sheet

* refactor: improve type checking

* fix: check value undefined

* fix: custom check for price

* test: remove CSV test

* test: remove CSV test

* fix: csv import dates

* test: change CSV

* chore: update example script

* chore: update docs script
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsErrors.xlsx
+++ b/examples/test/testFiles/TwoRowsErrors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\ui5-cc-excelUpload\examples\test\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13801231-C7C7-4AB4-AAFD-E743903776F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876206F6-6DEC-9141-8D92-C00756724018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="5820" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="4140" windowWidth="21600" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Product Test 1</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>WRONGCOLUMN[TEST]</t>
+  </si>
+  <si>
+    <t>05/14/2021</t>
+  </si>
+  <si>
+    <t>TIME</t>
   </si>
 </sst>
 </file>
@@ -522,17 +528,17 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:H1"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="9" max="9" width="17.875" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -561,7 +567,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>253</v>
       </c>
@@ -587,7 +593,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>253</v>
       </c>
@@ -613,7 +619,7 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>253</v>
       </c>
@@ -639,7 +645,7 @@
         <v>0.70833333333333304</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>253</v>
       </c>
@@ -665,7 +671,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>253</v>
       </c>
@@ -691,7 +697,7 @@
         <v>0.79166666666666696</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>2</v>
       </c>
@@ -714,7 +720,7 @@
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>253</v>
       </c>
@@ -740,7 +746,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>253</v>
       </c>
@@ -766,7 +772,7 @@
         <v>0.91666666666666696</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>253</v>
       </c>
@@ -792,7 +798,7 @@
         <v>0.95833333333333304</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>253</v>
       </c>
@@ -818,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>253</v>
       </c>
@@ -844,7 +850,7 @@
         <v>1.0416666666666701</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>253</v>
       </c>
@@ -870,7 +876,7 @@
         <v>1.0833333333333299</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>2</v>
       </c>
@@ -893,7 +899,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>253</v>
       </c>
@@ -919,7 +925,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>253</v>
       </c>
@@ -932,8 +938,8 @@
       <c r="D16">
         <v>26.56</v>
       </c>
-      <c r="E16" s="1">
-        <v>45255</v>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F16" s="1">
         <v>45254</v>
@@ -945,7 +951,7 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>253</v>
       </c>
@@ -971,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>253</v>
       </c>
@@ -997,7 +1003,7 @@
         <v>1.2916666666666701</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>253</v>
       </c>
@@ -1019,17 +1025,17 @@
       <c r="G19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H19">
-        <v>2.041666666666667</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>

</xml_diff>